<commit_message>
quantify y works w/ box plot
</commit_message>
<xml_diff>
--- a/code/latest/terms.xlsx
+++ b/code/latest/terms.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimd999/research/script_not_in_dropbox/srpAnalytics/analysis/latest/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimd999/research/script_not_in_dropbox/srpAnalytics/code/latest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783B22A8-DFE6-074D-89F7-356EBAD5E97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4939643-F6D1-7B42-9754-0731B43442A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1880" yWindow="460" windowWidth="15140" windowHeight="12920" xr2:uid="{F882FDEF-851F-DC4A-B978-FE9B8FD86AFC}"/>
+    <workbookView xWindow="1880" yWindow="460" windowWidth="21940" windowHeight="12920" xr2:uid="{F882FDEF-851F-DC4A-B978-FE9B8FD86AFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -262,7 +262,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -309,6 +309,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -330,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -353,7 +370,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -673,7 +693,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -986,15 +1006,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
+    <row r="29" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7" t="s">
+      <c r="B29" s="8"/>
+      <c r="C29" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="9" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>